<commit_message>
worked on OA processing script for RA presentations
</commit_message>
<xml_diff>
--- a/outputs/complete_lists/Older Adults/OA S002.xlsx
+++ b/outputs/complete_lists/Older Adults/OA S002.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Updates\Desktop\Alana\UA\R_projects\nav_room_project\outputs\complete_lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amuller\Desktop\Alana\UA\R_projects\inflatable-project\outputs\complete_lists\Older Adults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5962FD89-37E1-4161-AA72-941545D6149C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7754A05C-1E55-44EE-9524-E2523E091A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="220" windowWidth="22340" windowHeight="19860"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="17420" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ten_lists" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1313,11 +1313,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E5" sqref="E5:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1390,13 +1390,13 @@
         <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>36</v>
@@ -1416,13 +1416,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>52</v>
@@ -1442,13 +1442,13 @@
         <v>118</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>82</v>
@@ -1468,13 +1468,13 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>85</v>

</xml_diff>